<commit_message>
finish analysis, select results for writing
</commit_message>
<xml_diff>
--- a/data/Pythium_Azoxystrobin.xlsx
+++ b/data/Pythium_Azoxystrobin.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85BC624-F6E1-4DF3-B538-41849A657722}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C98F48-757E-40B3-8CEF-34647CC54715}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4560" yWindow="-15480" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -432,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H397"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2332,10 +2332,10 @@
         <v>3</v>
       </c>
       <c r="F73">
-        <v>37.83</v>
+        <v>10</v>
       </c>
       <c r="G73">
-        <v>37.81</v>
+        <v>0</v>
       </c>
       <c r="H73">
         <v>0</v>
@@ -10766,6 +10766,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H1" xr:uid="{04929DA8-B646-4953-AFDF-D1279F83E6FF}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>